<commit_message>
Full modification of the flow
</commit_message>
<xml_diff>
--- a/modules/parabole-module-ccar/Rule_Concept_Map.xlsx
+++ b/modules/parabole-module-ccar/Rule_Concept_Map.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sandbox\workspace\rda\parabole-solution-rda\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sandbox\workspace\rda_new\rda\parabole-solution-rda\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="7650"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,24 +21,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
-  <si>
-    <t>CRE PD Model</t>
-  </si>
-  <si>
-    <t>SME PD Model</t>
-  </si>
-  <si>
-    <t>Auto LGD Model</t>
-  </si>
-  <si>
-    <t>HE EAD Model</t>
-  </si>
-  <si>
-    <t>Auto LDG Model</t>
-  </si>
-  <si>
-    <t>23,25,21,31,7,50,10,49,41,43,21,36,25,11,44,14</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>Rule 1 is rule 1</t>
+  </si>
+  <si>
+    <t>Rule 2 is rule 2</t>
+  </si>
+  <si>
+    <t>CCAR1</t>
+  </si>
+  <si>
+    <t>CCAR2</t>
+  </si>
+  <si>
+    <t>3,4</t>
+  </si>
+  <si>
+    <t>1,2</t>
   </si>
 </sst>
 </file>
@@ -380,26 +380,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.140625" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="44.140625" customWidth="1"/>
-    <col min="4" max="4" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>34</v>
+        <v>76</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -410,49 +408,20 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>38</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>85</v>
-      </c>
-      <c r="B3" t="s">
         <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>85</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>